<commit_message>
first basic build ready
</commit_message>
<xml_diff>
--- a/tests/output/basic.xlsx
+++ b/tests/output/basic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Repos\cardlatex\tests\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Repos\cardlatex\tests\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC4E18B-07AC-429D-92F4-F004588A91D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6192D0-70FE-4192-AC0C-81404938BB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13815" yWindow="10890" windowWidth="15210" windowHeight="9825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
     <t>background</t>
   </si>
   <si>
-    <t>hello</t>
+    <t>hello2</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>